<commit_message>
Clarified information regarding auto-mode select
</commit_message>
<xml_diff>
--- a/Robot2015/Robot Class Checklist.xlsx
+++ b/Robot2015/Robot Class Checklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="25440" windowHeight="14370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -120,9 +120,6 @@
     <t>check</t>
   </si>
   <si>
-    <t>We might add a controller to choose Autonomi</t>
-  </si>
-  <si>
     <t>not tested</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>uses preferences</t>
+  </si>
+  <si>
+    <t>We have a controller to choose Autonomi, needs testing</t>
   </si>
 </sst>
 </file>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:F11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -594,7 +594,7 @@
         <v>ü</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F4" s="5"/>
     </row>
@@ -603,7 +603,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="2" t="str">
         <f t="shared" ref="D5:D35" si="0">IF(EXACT(LOWER(C5), "check"), "ü", "û")</f>
@@ -617,7 +617,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -631,7 +631,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -659,14 +659,14 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="5"/>
     </row>
@@ -689,14 +689,14 @@
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" s="5"/>
     </row>
@@ -705,14 +705,14 @@
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="5"/>
     </row>
@@ -721,14 +721,14 @@
         <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F13" s="5"/>
     </row>
@@ -737,7 +737,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="2" t="str">
         <f t="shared" si="0"/>
@@ -751,14 +751,14 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F15" s="5"/>
     </row>
@@ -767,14 +767,14 @@
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" s="5"/>
     </row>
@@ -783,14 +783,14 @@
         <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F17" s="5"/>
     </row>
@@ -799,7 +799,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="2" t="str">
         <f t="shared" si="0"/>
@@ -810,23 +810,23 @@
     </row>
     <row r="19" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>33</v>
@@ -840,23 +840,23 @@
     </row>
     <row r="21" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>33</v>
@@ -870,10 +870,10 @@
     </row>
     <row r="23" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" s="2" t="str">
         <f t="shared" si="0"/>
@@ -887,14 +887,14 @@
         <v>16</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F24" s="5"/>
     </row>
@@ -903,14 +903,14 @@
         <v>17</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>û</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="D25" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>û</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="F25" s="5"/>
     </row>
@@ -919,7 +919,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" s="2" t="str">
         <f t="shared" si="0"/>
@@ -933,7 +933,7 @@
         <v>19</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D27" s="2" t="str">
         <f t="shared" si="0"/>
@@ -947,7 +947,7 @@
         <v>20</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D28" s="2" t="str">
         <f t="shared" si="0"/>
@@ -961,7 +961,7 @@
         <v>21</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D29" s="2" t="str">
         <f t="shared" si="0"/>
@@ -989,14 +989,14 @@
         <v>23</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D31" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F31" s="5"/>
     </row>
@@ -1005,7 +1005,7 @@
         <v>24</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1019,7 +1019,7 @@
         <v>25</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D33" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1033,7 +1033,7 @@
         <v>26</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D34" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1047,7 +1047,7 @@
         <v>27</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D35" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1061,23 +1061,23 @@
         <v>32</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D36" s="2" t="str">
         <f>IF(EXACT(LOWER(C36), "check"), "ü", "û")</f>
         <v>û</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D37" s="2" t="str">
         <f>IF(EXACT(LOWER(C37), "check"), "ü", "û")</f>
@@ -1088,27 +1088,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E19:F19"/>
@@ -1125,6 +1104,27 @@
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E29:F29"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added the OI.html and made a formatting update to the checklist
The html is here so the drivers can view the controls of the robot even
when offline.
</commit_message>
<xml_diff>
--- a/Robot2015/Robot Class Checklist.xlsx
+++ b/Robot2015/Robot Class Checklist.xlsx
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -551,7 +551,7 @@
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1088,6 +1088,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E19:F19"/>
@@ -1104,27 +1125,6 @@
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E29:F29"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
The robot will drive backwards now
Sorry
</commit_message>
<xml_diff>
--- a/Robot2015/Robot Class Checklist.xlsx
+++ b/Robot2015/Robot Class Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
   <si>
     <t>Class</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>not completely tested</t>
+  </si>
+  <si>
+    <t>command to test the PID loops</t>
+  </si>
+  <si>
+    <t>elevator works, arm untested</t>
   </si>
 </sst>
 </file>
@@ -550,7 +556,7 @@
   <dimension ref="B1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -612,11 +618,11 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2" t="str">
         <f t="shared" ref="D5:D35" si="0">IF(EXACT(LOWER(C5), "check"), "ü", "û")</f>
-        <v>û</v>
+        <v>ü</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -626,11 +632,11 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>û</v>
+        <v>ü</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -640,11 +646,11 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>û</v>
+        <v>ü</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -657,7 +663,7 @@
         <v>33</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(EXACT(LOWER(C8), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -876,14 +882,14 @@
         <v>43</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ü</v>
+        <v>û</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F22" s="5"/>
     </row>
@@ -970,11 +976,11 @@
         <v>20</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>û</v>
+        <v>ü</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -990,7 +996,9 @@
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
-      <c r="E29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -1121,6 +1129,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E19:F19"/>
@@ -1137,27 +1166,6 @@
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E29:F29"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Named SlideWinder in the checklist as well
Also added vision and led
</commit_message>
<xml_diff>
--- a/Robot2015/Robot Class Checklist.xlsx
+++ b/Robot2015/Robot Class Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
   <si>
     <t>Class</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Preferences</t>
   </si>
   <si>
-    <t>Robot</t>
-  </si>
-  <si>
     <t>RobotMap</t>
   </si>
   <si>
@@ -51,12 +48,6 @@
     <t>AutoGrabRecycling</t>
   </si>
   <si>
-    <t>AutoModeONE_StackTotes</t>
-  </si>
-  <si>
-    <t>AutoModeTWO_TakeRecycling</t>
-  </si>
-  <si>
     <t>AutoSlideToLine</t>
   </si>
   <si>
@@ -178,6 +169,21 @@
   </si>
   <si>
     <t>elevator works, arm untested</t>
+  </si>
+  <si>
+    <t>Robot Vision</t>
+  </si>
+  <si>
+    <t>AutoModeOne_StackTotes</t>
+  </si>
+  <si>
+    <t>AutoModeTwo_TakeRecycling</t>
+  </si>
+  <si>
+    <t>SlideWinder</t>
+  </si>
+  <si>
+    <t>Robot LEDs</t>
   </si>
 </sst>
 </file>
@@ -553,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F37"/>
+  <dimension ref="B1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="E39" sqref="E39:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -572,7 +578,7 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -587,13 +593,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F3" s="6"/>
     </row>
@@ -602,14 +608,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>IF(EXACT(LOWER(C4), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F4" s="5"/>
     </row>
@@ -618,7 +624,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2" t="str">
         <f t="shared" ref="D5:D35" si="0">IF(EXACT(LOWER(C5), "check"), "ü", "û")</f>
@@ -632,7 +638,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -643,10 +649,10 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -657,106 +663,106 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>IF(EXACT(LOWER(C8), "check"), "ü", "û")</f>
         <v>ü</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D14" s="2" t="str">
         <f t="shared" si="0"/>
@@ -767,202 +773,202 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D27" s="2" t="str">
         <f t="shared" si="0"/>
@@ -973,10 +979,10 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D28" s="2" t="str">
         <f t="shared" si="0"/>
@@ -987,138 +993,138 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D29" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D30" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ü</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D31" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D32" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D33" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D35" s="2" t="str">
         <f t="shared" si="0"/>
         <v>û</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D36" s="2" t="str">
         <f>IF(EXACT(LOWER(C36), "check"), "ü", "û")</f>
         <v>û</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D37" s="2" t="str">
         <f>IF(EXACT(LOWER(C37), "check"), "ü", "û")</f>
@@ -1127,8 +1133,59 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="2" t="str">
+        <f>IF(EXACT(LOWER(C38), "check"), "ü", "û")</f>
+        <v>û</v>
+      </c>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="2" t="str">
+        <f>IF(EXACT(LOWER(C39), "check"), "ü", "û")</f>
+        <v>û</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="39">
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
@@ -1145,27 +1202,6 @@
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>